<commit_message>
this commit is a mistake
</commit_message>
<xml_diff>
--- a/dataset_tracking.xlsx
+++ b/dataset_tracking.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,17 +477,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>config-1.yml</t>
+          <t>dataset-config-001.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+          <t>n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -496,6 +496,38 @@
         </is>
       </c>
       <c r="F2" t="inlineStr">
+        <is>
+          <t>1,000,000 samples, 20 features, linear target</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dataset-config-002.yml</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>1,000,000 samples, 20 features, linear target</t>
         </is>
@@ -512,7 +544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,7 +622,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>config-1.yml</t>
+          <t>dataset-config-001.yml</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -603,10 +635,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
         <v>20</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -625,6 +657,52 @@
         </is>
       </c>
       <c r="L2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dataset-config-002.yml</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>42</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -639,7 +717,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,7 +775,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -726,7 +804,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -755,7 +833,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -784,7 +862,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -813,7 +891,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -842,7 +920,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -871,7 +949,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -900,7 +978,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -929,7 +1007,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -958,7 +1036,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -987,7 +1065,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1016,7 +1094,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1045,7 +1123,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1074,7 +1152,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1103,7 +1181,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1132,7 +1210,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1161,7 +1239,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1190,7 +1268,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1219,7 +1297,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1248,7 +1326,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>continuous</t>
+          <t>discrete</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1261,6 +1339,586 @@
         <v>0</v>
       </c>
       <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>feature_0</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>feature_1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-2.8</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>feature_2</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>feature_3</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>feature_4</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-4.1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>feature_5</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>15</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>feature_6</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>feature_7</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>feature_8</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>feature_9</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>12</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>feature_10</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-3.3</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>feature_11</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>8</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>feature_12</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>feature_13</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>20</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>feature_14</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>feature_15</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>7</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-5</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>feature_16</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>feature_17</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>25</v>
+      </c>
+      <c r="E39" t="n">
+        <v>5</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>feature_18</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>-12</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-1.6</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>feature_19</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>discrete</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>18</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1275,7 +1933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1350,6 +2008,34 @@
         <v>5.2</v>
       </c>
       <c r="H2" t="n">
+        <v>10.2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="H3" t="n">
         <v>10.2</v>
       </c>
     </row>
@@ -1364,7 +2050,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1417,30 +2103,65 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>configs\data_generation\config-1.yml</t>
+          <t>configs\data_generation\dataset-config-001.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>data\n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+          <t>data\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>reports\figures\n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+          <t>reports\figures\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>379.1</v>
+        <v>106.1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>04111418c3</t>
+          <t>f938398f95</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Linear function, 20C/0D features</t>
+          <t>Linear function, 0C/20D features</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>configs\data_generation\dataset-config-002.yml</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>data\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>reports\figures\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>106.1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>f938398f95</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Linear function, 0C/20D features</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented dataset tracking in a spreadsheet
</commit_message>
<xml_diff>
--- a/dataset_tracking.xlsx
+++ b/dataset_tracking.xlsx
@@ -477,7 +477,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dataset-config-001.yml</t>
+          <t>config-1.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -487,7 +487,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -509,17 +509,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dataset-config-002.yml</t>
+          <t>config-2.yml</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+          <t>n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dataset-config-001.yml</t>
+          <t>config-1.yml</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -668,7 +668,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dataset-config-002.yml</t>
+          <t>config-2.yml</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -681,10 +681,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
         <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>20</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>discrete</t>
+          <t>continuous</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>configs\data_generation\dataset-config-001.yml</t>
+          <t>configs\data_generation\config-1.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2138,30 +2138,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>configs\data_generation\dataset-config-002.yml</t>
+          <t>configs\data_generation\config-2.yml</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>data\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+          <t>data\n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>reports\figures\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+          <t>reports\figures\n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>106.1</v>
+        <v>379.1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>f938398f95</t>
+          <t>04111418c3</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Linear function, 0C/20D features</t>
+          <t>Linear function, 20C/0D features</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
separated combined config into data generation and training configs
</commit_message>
<xml_diff>
--- a/dataset_tracking.xlsx
+++ b/dataset_tracking.xlsx
@@ -477,7 +477,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>config-1.yml</t>
+          <t>data-gen-config-001.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>config-2.yml</t>
+          <t>data-gen-config-002.yml</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>config-1.yml</t>
+          <t>data-gen-config-001.yml</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -668,7 +668,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>config-2.yml</t>
+          <t>data-gen-config-002.yml</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>configs\data_generation\config-1.yml</t>
+          <t>configs\data_generation\data-gen-config-001.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>configs\data_generation\config-2.yml</t>
+          <t>configs\data_generation\data-gen-config-002.yml</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">

</xml_diff>

<commit_message>
successfully generated datasets for 5,10,15,20 features
</commit_message>
<xml_diff>
--- a/dataset_tracking.xlsx
+++ b/dataset_tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\masters-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9D851C-0C5F-4311-B886-91F04492DAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107D6EBB-DEEC-4F2C-B61C-2048C2C12DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25770" yWindow="5130" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="5520" windowWidth="23430" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Registry" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="129">
   <si>
     <t>Dataset ID</t>
   </si>
@@ -47,28 +47,91 @@
     <t>DS001</t>
   </si>
   <si>
-    <t>data-config-002.yml</t>
+    <t>n1000000_f_init10_cont0_disc10_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>n1000000_f_init10_cont0_disc10_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>2025-07-03</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>1,000,000 samples, 10 features, linear target</t>
+  </si>
+  <si>
+    <t>DS002</t>
+  </si>
+  <si>
+    <t>n1000000_f_init10_cont10_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>n1000000_f_init10_cont10_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>DS003</t>
+  </si>
+  <si>
+    <t>n1000000_f_init15_cont0_disc15_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>n1000000_f_init15_cont0_disc15_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>1,000,000 samples, 15 features, linear target</t>
+  </si>
+  <si>
+    <t>DS004</t>
+  </si>
+  <si>
+    <t>n1000000_f_init15_cont15_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>n1000000_f_init15_cont15_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>DS005</t>
+  </si>
+  <si>
+    <t>n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>1,000,000 samples, 20 features, linear target</t>
+  </si>
+  <si>
+    <t>DS006</t>
+  </si>
+  <si>
+    <t>n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
   </si>
   <si>
     <t>n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
   </si>
   <si>
-    <t>2025-07-03</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>1,000,000 samples, 20 features, linear target</t>
-  </si>
-  <si>
-    <t>DS002</t>
-  </si>
-  <si>
-    <t>n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
-  </si>
-  <si>
-    <t>n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+    <t>DS007</t>
+  </si>
+  <si>
+    <t>n1000000_f_init5_cont0_disc5_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>n1000000_f_init5_cont0_disc5_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>1,000,000 samples, 5 features, linear target</t>
+  </si>
+  <si>
+    <t>DS008</t>
+  </si>
+  <si>
+    <t>n1000000_f_init5_cont5_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>n1000000_f_init5_cont5_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
   </si>
   <si>
     <t>Random Seed</t>
@@ -128,36 +191,39 @@
     <t>feature_0</t>
   </si>
   <si>
+    <t>discrete</t>
+  </si>
+  <si>
+    <t>feature_1</t>
+  </si>
+  <si>
+    <t>feature_2</t>
+  </si>
+  <si>
+    <t>feature_3</t>
+  </si>
+  <si>
+    <t>feature_4</t>
+  </si>
+  <si>
+    <t>feature_5</t>
+  </si>
+  <si>
+    <t>feature_6</t>
+  </si>
+  <si>
+    <t>feature_7</t>
+  </si>
+  <si>
+    <t>feature_8</t>
+  </si>
+  <si>
+    <t>feature_9</t>
+  </si>
+  <si>
     <t>continuous</t>
   </si>
   <si>
-    <t>feature_1</t>
-  </si>
-  <si>
-    <t>feature_2</t>
-  </si>
-  <si>
-    <t>feature_3</t>
-  </si>
-  <si>
-    <t>feature_4</t>
-  </si>
-  <si>
-    <t>feature_5</t>
-  </si>
-  <si>
-    <t>feature_6</t>
-  </si>
-  <si>
-    <t>feature_7</t>
-  </si>
-  <si>
-    <t>feature_8</t>
-  </si>
-  <si>
-    <t>feature_9</t>
-  </si>
-  <si>
     <t>feature_10</t>
   </si>
   <si>
@@ -188,9 +254,6 @@
     <t>feature_19</t>
   </si>
   <si>
-    <t>discrete</t>
-  </si>
-  <si>
     <t>Total Weights</t>
   </si>
   <si>
@@ -230,7 +293,82 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>configs\data_generation\data-config-002.yml</t>
+    <t>configs\data_generation\n1000000_f_init10_cont0_disc10_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>data\n1000000_f_init10_cont0_disc10_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>reports\figures\n1000000_f_init10_cont0_disc10_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+  </si>
+  <si>
+    <t>235d3f6928</t>
+  </si>
+  <si>
+    <t>Linear function, 0C/10D features</t>
+  </si>
+  <si>
+    <t>configs\data_generation\n1000000_f_init10_cont10_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>data\n1000000_f_init10_cont10_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>reports\figures\n1000000_f_init10_cont10_disc0_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+  </si>
+  <si>
+    <t>f976f4dd97</t>
+  </si>
+  <si>
+    <t>Linear function, 10C/0D features</t>
+  </si>
+  <si>
+    <t>configs\data_generation\n1000000_f_init15_cont0_disc15_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>data\n1000000_f_init15_cont0_disc15_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>reports\figures\n1000000_f_init15_cont0_disc15_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+  </si>
+  <si>
+    <t>28db5f7672</t>
+  </si>
+  <si>
+    <t>Linear function, 0C/15D features</t>
+  </si>
+  <si>
+    <t>configs\data_generation\n1000000_f_init15_cont15_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>data\n1000000_f_init15_cont15_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>reports\figures\n1000000_f_init15_cont15_disc0_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+  </si>
+  <si>
+    <t>2181ba0dac</t>
+  </si>
+  <si>
+    <t>Linear function, 15C/0D features</t>
+  </si>
+  <si>
+    <t>configs\data_generation\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>data\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>reports\figures\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+  </si>
+  <si>
+    <t>f938398f95</t>
+  </si>
+  <si>
+    <t>Linear function, 0C/20D features</t>
+  </si>
+  <si>
+    <t>configs\data_generation\n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
   </si>
   <si>
     <t>data\n1000000_f_init20_cont20_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
@@ -245,19 +383,34 @@
     <t>Linear function, 20C/0D features</t>
   </si>
   <si>
-    <t>configs\data_generation\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
-  </si>
-  <si>
-    <t>data\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
-  </si>
-  <si>
-    <t>reports\figures\n1000000_f_init20_cont0_disc20_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
-  </si>
-  <si>
-    <t>f938398f95</t>
-  </si>
-  <si>
-    <t>Linear function, 0C/20D features</t>
+    <t>configs\data_generation\n1000000_f_init5_cont0_disc5_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>data\n1000000_f_init5_cont0_disc5_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>reports\figures\n1000000_f_init5_cont0_disc5_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+  </si>
+  <si>
+    <t>fc8c86f74a</t>
+  </si>
+  <si>
+    <t>Linear function, 0C/5D features</t>
+  </si>
+  <si>
+    <t>configs\data_generation\n1000000_f_init5_cont5_disc0_add0_pert-none_scl0_func-linear_noise0_config.yml</t>
+  </si>
+  <si>
+    <t>data\n1000000_f_init5_cont5_disc0_add0_pert-none_scl0_func-linear_noise0_dataset.csv</t>
+  </si>
+  <si>
+    <t>reports\figures\n1000000_f_init5_cont5_disc0_add0_pert-none_scl0_func-linear_noise0_plot.pdf</t>
+  </si>
+  <si>
+    <t>32af596033</t>
+  </si>
+  <si>
+    <t>Linear function, 5C/0D features</t>
   </si>
 </sst>
 </file>
@@ -620,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,6 +849,126 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -703,10 +976,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,34 +1006,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -777,16 +1050,16 @@
         <v>1000000</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -795,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -815,27 +1088,255 @@
         <v>1000000</v>
       </c>
       <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>1000000</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="C5">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>1000000</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>1000000</v>
+      </c>
+      <c r="E6">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="L3">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>1000000</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>1000000</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>1000000</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9">
         <v>0</v>
       </c>
     </row>
@@ -846,7 +1347,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1048576"/>
@@ -868,22 +1369,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -891,10 +1392,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -914,10 +1415,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>-5</v>
@@ -937,10 +1438,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -960,10 +1461,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -983,10 +1484,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>-2</v>
@@ -1006,10 +1507,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -1029,10 +1530,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>-8</v>
@@ -1052,10 +1553,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1075,10 +1576,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>-1</v>
@@ -1098,10 +1599,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D11">
         <v>12</v>
@@ -1118,22 +1619,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D12">
-        <v>-6</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>-3.3</v>
+        <v>3.5</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1141,22 +1642,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>-5</v>
       </c>
       <c r="E13">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="F13">
-        <v>0.4</v>
+        <v>-2.8</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1164,22 +1665,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D14">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1.1000000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="F14">
-        <v>4.5999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1187,22 +1688,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>-0.9</v>
+        <v>5.2</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -1210,22 +1711,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D16">
-        <v>-10</v>
+        <v>-2</v>
       </c>
       <c r="E16">
-        <v>2.5</v>
+        <v>0.8</v>
       </c>
       <c r="F16">
-        <v>2.1</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -1233,22 +1734,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E17">
-        <v>1.6</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>-5</v>
+        <v>1.7</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -1256,22 +1757,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D18">
-        <v>-4</v>
+        <v>-8</v>
       </c>
       <c r="E18">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F18">
-        <v>0.3</v>
+        <v>-0.05</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -1279,22 +1780,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D19">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>1.8</v>
       </c>
       <c r="F19">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -1302,22 +1803,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D20">
-        <v>-12</v>
+        <v>-1</v>
       </c>
       <c r="E20">
-        <v>3.2</v>
+        <v>0.9</v>
       </c>
       <c r="F20">
-        <v>-1.6</v>
+        <v>-1.2</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -1325,22 +1826,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D21">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -1348,13 +1849,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -1371,13 +1872,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D23">
         <v>-5</v>
@@ -1394,13 +1895,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1417,13 +1918,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1440,13 +1941,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D26">
         <v>-2</v>
@@ -1463,13 +1964,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27">
         <v>15</v>
@@ -1486,13 +1987,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28">
         <v>-8</v>
@@ -1509,13 +2010,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1532,13 +2033,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D30">
         <v>-1</v>
@@ -1555,13 +2056,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D31">
         <v>12</v>
@@ -1578,13 +2079,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D32">
         <v>-6</v>
@@ -1601,13 +2102,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D33">
         <v>8</v>
@@ -1624,13 +2125,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D34">
         <v>-3</v>
@@ -1647,13 +2148,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D35">
         <v>20</v>
@@ -1670,13 +2171,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D36">
         <v>-10</v>
@@ -1693,22 +2194,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E37">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>-5</v>
+        <v>3.5</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1716,22 +2217,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D38">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="E38">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F38">
-        <v>0.3</v>
+        <v>-2.8</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -1739,22 +2240,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D39">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="F39">
-        <v>3.8</v>
+        <v>0.1</v>
       </c>
       <c r="G39" t="b">
         <v>1</v>
@@ -1762,22 +2263,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D40">
-        <v>-12</v>
+        <v>3</v>
       </c>
       <c r="E40">
-        <v>3.2</v>
+        <v>1</v>
       </c>
       <c r="F40">
-        <v>-1.6</v>
+        <v>5.2</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -1785,24 +2286,1404 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41">
+        <v>-2</v>
+      </c>
+      <c r="E41">
+        <v>0.8</v>
+      </c>
+      <c r="F41">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42">
+        <v>15</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>1.7</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>-8</v>
+      </c>
+      <c r="E43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F43">
+        <v>-0.05</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>1.8</v>
+      </c>
+      <c r="F44">
+        <v>2.9</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45">
+        <v>-1</v>
+      </c>
+      <c r="E45">
+        <v>0.9</v>
+      </c>
+      <c r="F45">
+        <v>-1.2</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46">
         <v>12</v>
       </c>
-      <c r="B41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="E46">
+        <v>2.8</v>
+      </c>
+      <c r="F46">
+        <v>0.8</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47">
+        <v>-6</v>
+      </c>
+      <c r="E47">
+        <v>1.3</v>
+      </c>
+      <c r="F47">
+        <v>-3.3</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <v>2.1</v>
+      </c>
+      <c r="F48">
+        <v>0.4</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49">
+        <v>-3</v>
+      </c>
+      <c r="E49">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F49">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50">
+        <v>20</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>-0.9</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51">
+        <v>-10</v>
+      </c>
+      <c r="E51">
+        <v>2.5</v>
+      </c>
+      <c r="F51">
+        <v>2.1</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
         <v>54</v>
       </c>
-      <c r="D41">
+      <c r="C52" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>3.5</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53">
+        <v>-5</v>
+      </c>
+      <c r="E53">
+        <v>1.5</v>
+      </c>
+      <c r="F53">
+        <v>-2.8</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>2.5</v>
+      </c>
+      <c r="F54">
+        <v>0.1</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>5.2</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56">
+        <v>-2</v>
+      </c>
+      <c r="E56">
+        <v>0.8</v>
+      </c>
+      <c r="F56">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57">
+        <v>15</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>1.7</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58">
+        <v>-8</v>
+      </c>
+      <c r="E58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F58">
+        <v>-0.05</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>1.8</v>
+      </c>
+      <c r="F59">
+        <v>2.9</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60">
+        <v>-1</v>
+      </c>
+      <c r="E60">
+        <v>0.9</v>
+      </c>
+      <c r="F60">
+        <v>-1.2</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61">
+        <v>12</v>
+      </c>
+      <c r="E61">
+        <v>2.8</v>
+      </c>
+      <c r="F61">
+        <v>0.8</v>
+      </c>
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" t="s">
+        <v>55</v>
+      </c>
+      <c r="D62">
+        <v>-6</v>
+      </c>
+      <c r="E62">
+        <v>1.3</v>
+      </c>
+      <c r="F62">
+        <v>-3.3</v>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63">
+        <v>8</v>
+      </c>
+      <c r="E63">
+        <v>2.1</v>
+      </c>
+      <c r="F63">
+        <v>0.4</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64">
+        <v>-3</v>
+      </c>
+      <c r="E64">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F64">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65">
+        <v>20</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>-0.9</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66">
+        <v>-10</v>
+      </c>
+      <c r="E66">
+        <v>2.5</v>
+      </c>
+      <c r="F66">
+        <v>2.1</v>
+      </c>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>55</v>
+      </c>
+      <c r="D67">
+        <v>7</v>
+      </c>
+      <c r="E67">
+        <v>1.6</v>
+      </c>
+      <c r="F67">
+        <v>-5</v>
+      </c>
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68">
+        <v>-4</v>
+      </c>
+      <c r="E68">
+        <v>1.4</v>
+      </c>
+      <c r="F68">
+        <v>0.3</v>
+      </c>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69">
+        <v>25</v>
+      </c>
+      <c r="E69">
+        <v>5</v>
+      </c>
+      <c r="F69">
+        <v>3.8</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70">
+        <v>-12</v>
+      </c>
+      <c r="E70">
+        <v>3.2</v>
+      </c>
+      <c r="F70">
+        <v>-1.6</v>
+      </c>
+      <c r="G70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71">
         <v>18</v>
       </c>
-      <c r="E41">
+      <c r="E71">
         <v>3.8</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41" t="b">
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72">
+        <v>3.5</v>
+      </c>
+      <c r="G72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73">
+        <v>-5</v>
+      </c>
+      <c r="E73">
+        <v>1.5</v>
+      </c>
+      <c r="F73">
+        <v>-2.8</v>
+      </c>
+      <c r="G73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>2.5</v>
+      </c>
+      <c r="F74">
+        <v>0.1</v>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" t="s">
+        <v>58</v>
+      </c>
+      <c r="C75" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>5.2</v>
+      </c>
+      <c r="G75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76">
+        <v>-2</v>
+      </c>
+      <c r="E76">
+        <v>0.8</v>
+      </c>
+      <c r="F76">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77">
+        <v>15</v>
+      </c>
+      <c r="E77">
+        <v>3</v>
+      </c>
+      <c r="F77">
+        <v>1.7</v>
+      </c>
+      <c r="G77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78" t="s">
+        <v>65</v>
+      </c>
+      <c r="D78">
+        <v>-8</v>
+      </c>
+      <c r="E78">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F78">
+        <v>-0.05</v>
+      </c>
+      <c r="G78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79">
+        <v>5</v>
+      </c>
+      <c r="E79">
+        <v>1.8</v>
+      </c>
+      <c r="F79">
+        <v>2.9</v>
+      </c>
+      <c r="G79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" t="s">
+        <v>65</v>
+      </c>
+      <c r="D80">
+        <v>-1</v>
+      </c>
+      <c r="E80">
+        <v>0.9</v>
+      </c>
+      <c r="F80">
+        <v>-1.2</v>
+      </c>
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" t="s">
+        <v>65</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+      <c r="E81">
+        <v>2.8</v>
+      </c>
+      <c r="F81">
+        <v>0.8</v>
+      </c>
+      <c r="G81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" t="s">
+        <v>66</v>
+      </c>
+      <c r="C82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82">
+        <v>-6</v>
+      </c>
+      <c r="E82">
+        <v>1.3</v>
+      </c>
+      <c r="F82">
+        <v>-3.3</v>
+      </c>
+      <c r="G82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83">
+        <v>8</v>
+      </c>
+      <c r="E83">
+        <v>2.1</v>
+      </c>
+      <c r="F83">
+        <v>0.4</v>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" t="s">
+        <v>68</v>
+      </c>
+      <c r="C84" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84">
+        <v>-3</v>
+      </c>
+      <c r="E84">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F84">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" t="s">
+        <v>69</v>
+      </c>
+      <c r="C85" t="s">
+        <v>65</v>
+      </c>
+      <c r="D85">
+        <v>20</v>
+      </c>
+      <c r="E85">
+        <v>4</v>
+      </c>
+      <c r="F85">
+        <v>-0.9</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" t="s">
+        <v>65</v>
+      </c>
+      <c r="D86">
+        <v>-10</v>
+      </c>
+      <c r="E86">
+        <v>2.5</v>
+      </c>
+      <c r="F86">
+        <v>2.1</v>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" t="s">
+        <v>65</v>
+      </c>
+      <c r="D87">
+        <v>7</v>
+      </c>
+      <c r="E87">
+        <v>1.6</v>
+      </c>
+      <c r="F87">
+        <v>-5</v>
+      </c>
+      <c r="G87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" t="s">
+        <v>72</v>
+      </c>
+      <c r="C88" t="s">
+        <v>65</v>
+      </c>
+      <c r="D88">
+        <v>-4</v>
+      </c>
+      <c r="E88">
+        <v>1.4</v>
+      </c>
+      <c r="F88">
+        <v>0.3</v>
+      </c>
+      <c r="G88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" t="s">
+        <v>65</v>
+      </c>
+      <c r="D89">
+        <v>25</v>
+      </c>
+      <c r="E89">
+        <v>5</v>
+      </c>
+      <c r="F89">
+        <v>3.8</v>
+      </c>
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C90" t="s">
+        <v>65</v>
+      </c>
+      <c r="D90">
+        <v>-12</v>
+      </c>
+      <c r="E90">
+        <v>3.2</v>
+      </c>
+      <c r="F90">
+        <v>-1.6</v>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" t="s">
+        <v>75</v>
+      </c>
+      <c r="C91" t="s">
+        <v>65</v>
+      </c>
+      <c r="D91">
+        <v>18</v>
+      </c>
+      <c r="E91">
+        <v>3.8</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>29</v>
+      </c>
+      <c r="B92" t="s">
+        <v>54</v>
+      </c>
+      <c r="C92" t="s">
+        <v>55</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92">
+        <v>3.5</v>
+      </c>
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" t="s">
+        <v>56</v>
+      </c>
+      <c r="C93" t="s">
+        <v>55</v>
+      </c>
+      <c r="D93">
+        <v>-5</v>
+      </c>
+      <c r="E93">
+        <v>1.5</v>
+      </c>
+      <c r="F93">
+        <v>-2.8</v>
+      </c>
+      <c r="G93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94" t="s">
+        <v>57</v>
+      </c>
+      <c r="C94" t="s">
+        <v>55</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>2.5</v>
+      </c>
+      <c r="F94">
+        <v>0.1</v>
+      </c>
+      <c r="G94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>29</v>
+      </c>
+      <c r="B95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C95" t="s">
+        <v>55</v>
+      </c>
+      <c r="D95">
+        <v>3</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>5.2</v>
+      </c>
+      <c r="G95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>29</v>
+      </c>
+      <c r="B96" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" t="s">
+        <v>55</v>
+      </c>
+      <c r="D96">
+        <v>-2</v>
+      </c>
+      <c r="E96">
+        <v>0.8</v>
+      </c>
+      <c r="F96">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" t="s">
+        <v>54</v>
+      </c>
+      <c r="C97" t="s">
+        <v>65</v>
+      </c>
+      <c r="D97">
+        <v>10</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <v>3.5</v>
+      </c>
+      <c r="G97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>33</v>
+      </c>
+      <c r="B98" t="s">
+        <v>56</v>
+      </c>
+      <c r="C98" t="s">
+        <v>65</v>
+      </c>
+      <c r="D98">
+        <v>-5</v>
+      </c>
+      <c r="E98">
+        <v>1.5</v>
+      </c>
+      <c r="F98">
+        <v>-2.8</v>
+      </c>
+      <c r="G98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>33</v>
+      </c>
+      <c r="B99" t="s">
+        <v>57</v>
+      </c>
+      <c r="C99" t="s">
+        <v>65</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>2.5</v>
+      </c>
+      <c r="F99">
+        <v>0.1</v>
+      </c>
+      <c r="G99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>33</v>
+      </c>
+      <c r="B100" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" t="s">
+        <v>65</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>5.2</v>
+      </c>
+      <c r="G100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>33</v>
+      </c>
+      <c r="B101" t="s">
+        <v>59</v>
+      </c>
+      <c r="C101" t="s">
+        <v>65</v>
+      </c>
+      <c r="D101">
+        <v>-2</v>
+      </c>
+      <c r="E101">
+        <v>0.8</v>
+      </c>
+      <c r="F101">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G101" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1813,10 +3694,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,25 +3717,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1862,25 +3743,25 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>-5</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="G2">
         <v>5.2</v>
       </c>
       <c r="H2">
-        <v>10.199999999999999</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1888,25 +3769,181 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>-5</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="G3">
         <v>5.2</v>
       </c>
       <c r="H3">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G4">
+        <v>5.2</v>
+      </c>
+      <c r="H4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G5">
+        <v>5.2</v>
+      </c>
+      <c r="H5">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>-5</v>
+      </c>
+      <c r="G6">
+        <v>5.2</v>
+      </c>
+      <c r="H6">
         <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>-5</v>
+      </c>
+      <c r="G7">
+        <v>5.2</v>
+      </c>
+      <c r="H7">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G8">
+        <v>5.2</v>
+      </c>
+      <c r="H8">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="G9">
+        <v>5.2</v>
+      </c>
+      <c r="H9">
+        <v>9.3000000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -1916,10 +3953,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +3966,7 @@
     <col min="3" max="3" width="84.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="91.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1938,22 +3975,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1961,22 +3998,22 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E2">
-        <v>379.1</v>
+        <v>57.1</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1984,22 +4021,160 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E3">
+        <v>199.3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4">
+        <v>83.6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5">
+        <v>289</v>
+      </c>
+      <c r="F5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6">
         <v>106.1</v>
       </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>77</v>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7">
+        <v>379.1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8">
+        <v>31.6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9">
+        <v>108.5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spreadsheet tracker now checks for deleted datasets as well as new ones and removes them from the spreadsheet
</commit_message>
<xml_diff>
--- a/dataset_tracking.xlsx
+++ b/dataset_tracking.xlsx
@@ -466,17 +466,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>n10000_f_init5_cont0_disc5_sep6p6_config.yml</t>
+          <t>n10000_f_init5_cont0_disc5_sep6p6_seed42_config.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>n10000_f_init5_cont0_disc5_sep6p6_dataset.csv</t>
+          <t>n10000_f_init5_cont0_disc5_sep6p6_seed42_dataset.csv</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>n10000_f_init5_cont0_disc5_sep6p6_config.yml</t>
+          <t>n10000_f_init5_cont0_disc5_sep6p6_seed42_config.yml</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -645,7 +645,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -677,7 +677,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -709,7 +709,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -741,7 +741,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -773,7 +773,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -851,17 +851,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DS001</t>
+          <t>DS002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>configs/data_generation/n10000_f_init5_cont0_disc5_sep6p6_config.yml</t>
+          <t>configs/data_generation/n10000_f_init5_cont0_disc5_sep6p6_seed42_config.yml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>data/n10000_f_init5_cont0_disc5_sep6p6_dataset.csv</t>
+          <t>data/n10000_f_init5_cont0_disc5_sep6p6_seed42_dataset.csv</t>
         </is>
       </c>
       <c r="D2" t="n">

</xml_diff>

<commit_message>
added multi seed data gen and training
</commit_message>
<xml_diff>
--- a/dataset_tracking.xlsx
+++ b/dataset_tracking.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,27 +466,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed4_config.yml</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed4_dataset.csv</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1,000,000 samples, 5 features, Avg. Sep: 5.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>DS002</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>n10000_f_init5_cont0_disc5_sep6p6_seed42_config.yml</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>n10000_f_init5_cont0_disc5_sep6p6_seed42_dataset.csv</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-07-24</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>10,000 samples, 5 features, Avg. Sep: 6.60</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed0_config.yml</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed0_dataset.csv</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1,000,000 samples, 5 features, Avg. Sep: 5.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed1_config.yml</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed1_dataset.csv</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1,000,000 samples, 5 features, Avg. Sep: 5.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed3_config.yml</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed3_dataset.csv</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1,000,000 samples, 5 features, Avg. Sep: 5.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed2_config.yml</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>n1000000_f_init5_cont0_disc5_sep5p1_seed2_dataset.csv</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1,000,000 samples, 5 features, Avg. Sep: 5.10</t>
         </is>
       </c>
     </row>
@@ -501,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,36 +657,6 @@
         <is>
           <t>avg_separation</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>DS002</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>n10000_f_init5_cont0_disc5_sep6p6_seed42_config.yml</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>42</v>
-      </c>
-      <c r="D2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2" t="n">
-        <v>6.6</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -640,166 +718,6 @@
         <is>
           <t>Mean Separation</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>DS002</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>feature_0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>discrete</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DS002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>feature_1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>discrete</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>-3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="H3" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DS002</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>feature_2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>discrete</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>DS002</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>feature_3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>discrete</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>-2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>DS002</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>feature_4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>discrete</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="H6" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -813,7 +731,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -848,31 +766,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>DS002</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>configs/data_generation/n10000_f_init5_cont0_disc5_sep6p6_seed42_config.yml</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>data/n10000_f_init5_cont0_disc5_sep6p6_seed42_dataset.csv</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2ca41b89b7</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
huge overhall of file management. all run scripts aggregated into modules in src
</commit_message>
<xml_diff>
--- a/dataset_tracking.xlsx
+++ b/dataset_tracking.xlsx
@@ -609,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,38 +625,98 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Config File</t>
+          <t>Random Seed</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Random Seed</t>
+          <t>Num Samples</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>n_samples</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>n_features</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>continuous_features</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>discrete_features</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>avg_separation</t>
-        </is>
+          <t>Num Initial Features</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,33 +751,703 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Feature Type</t>
+          <t>Signal Mean</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Signal Mean</t>
+          <t>Noise Mean</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Separation</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Signal Std</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Noise Mean</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Noise Std</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Mean Separation</t>
-        </is>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>feature_0</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>feature_1</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>feature_2</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>feature_3</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>feature_4</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>feature_0</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>feature_1</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>feature_2</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>feature_3</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>feature_4</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>feature_0</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>7</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>7</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>feature_1</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>feature_2</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>6</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>feature_3</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>feature_4</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>feature_0</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>7</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>feature_1</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" t="n">
+        <v>7</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>feature_2</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>feature_3</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>feature_4</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>feature_0</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>7</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>7</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>feature_1</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" t="n">
+        <v>7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>feature_2</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>6</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>feature_3</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>feature_4</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.8</v>
       </c>
     </row>
   </sheetData>
@@ -731,7 +1461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -747,22 +1477,117 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Config Path</t>
+          <t>File Size (MB)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Dataset Path</t>
+          <t>MD5 Checksum</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>File Size (MB)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Checksum (MD5)</t>
+          <t>Full Path</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DS001</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>22.42</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>b52460d410</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>/home/jovyan/masters-project/data/n1000000_f_init5_cont0_disc5_sep5p1_seed4_dataset.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS002</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>22.42</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>9b9b540b13</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>/home/jovyan/masters-project/data/n1000000_f_init5_cont0_disc5_sep5p1_seed0_dataset.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DS003</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>22.42</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>964f876ea1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>/home/jovyan/masters-project/data/n1000000_f_init5_cont0_disc5_sep5p1_seed1_dataset.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DS004</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>22.42</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dda806b1d5</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>/home/jovyan/masters-project/data/n1000000_f_init5_cont0_disc5_sep5p1_seed3_dataset.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DS005</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>22.42</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>9f6a91c6a8</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>/home/jovyan/masters-project/data/n1000000_f_init5_cont0_disc5_sep5p1_seed2_dataset.csv</t>
         </is>
       </c>
     </row>

</xml_diff>